<commit_message>
Added Teyvat Archives API Workflow and Schema
</commit_message>
<xml_diff>
--- a/Genshin Impact Character Builder/TeyvatArchives_Schema.xlsx
+++ b/Genshin Impact Character Builder/TeyvatArchives_Schema.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RED\ITECC05repos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RED\ITECC05repos\MovieVerse\Genshin Impact Character Builder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5609389D-3D83-4368-B0B2-D10E7160BC88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22970DBD-3FF3-4D43-81D7-0852E824AC6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{006D6FF3-F200-409E-AB9B-33BD2B714723}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{006D6FF3-F200-409E-AB9B-33BD2B714723}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="173">
   <si>
     <t>Key</t>
   </si>
@@ -1115,7 +1115,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1136,9 +1136,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1475,7 +1472,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9E36478-E851-4AD7-8461-CF6C9F6A9948}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="91" workbookViewId="0">
+    <sheetView zoomScale="91" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -1658,7 +1655,7 @@
       <c r="B7" s="1"/>
       <c r="C7" s="6"/>
       <c r="D7" s="5"/>
-      <c r="E7" s="8"/>
+      <c r="E7" s="5"/>
       <c r="F7" s="1"/>
       <c r="G7" s="4" t="s">
         <v>40</v>
@@ -1763,10 +1760,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0103C1D-6FB8-4FEA-A76A-FDDF11139D18}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1969,10 +1966,10 @@
     </row>
     <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D8" s="4" t="s">
-        <v>20</v>
+        <v>102</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>21</v>
+        <v>103</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>149</v>
@@ -1989,9 +1986,17 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D10" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2435,7 +2440,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:J1"/>
+      <selection activeCell="D6" sqref="D6:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>